<commit_message>
Adding the correct spreadsheet
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Applications" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="PrivateApp" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t xml:space="preserve">app_name</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">port</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
+    <t xml:space="preserve">protocol</t>
   </si>
   <si>
     <t xml:space="preserve">publisher_id</t>
@@ -40,7 +40,19 @@
     <t xml:space="preserve">publisher_name</t>
   </si>
   <si>
-    <t xml:space="preserve">testeAPI</t>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_publisher_dns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clientless_access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private_app_protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testeAPI2</t>
   </si>
   <si>
     <t xml:space="preserve">webserver.local</t>
@@ -50,16 +62,63 @@
   </si>
   <si>
     <t xml:space="preserve">Azure-Publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">webserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APIteste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server.local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">servers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vdi.local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.201.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.3.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;VERDADEIRO&quot;;&quot;VERDADEIRO&quot;;&quot;FALSO&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,9 +143,17 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,16 +198,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,61 +483,216 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>443</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating a Hashmap, so i dont need to put Publisher's ID on the spreadsheet
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t xml:space="preserve">app_name</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">publisher_id</t>
   </si>
   <si>
     <t xml:space="preserve">publisher_name</t>
@@ -483,10 +480,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,12 +492,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,177 +519,159 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>16</v>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>16</v>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>443</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>16</v>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new feature Update
</commit_message>
<xml_diff>
--- a/applications.xlsx
+++ b/applications.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t xml:space="preserve">app_name</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">192.168.3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">443,80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine,servers</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,7 +503,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,8 +658,8 @@
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>443</v>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -662,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>15</v>

</xml_diff>